<commit_message>
Add the RLS_thermal_v2.py for new soc and ocv value there is still some problem and its okey to improve
</commit_message>
<xml_diff>
--- a/data/Lab2_data/RLS/hppc_18650_p25_sococv.xlsx
+++ b/data/Lab2_data/RLS/hppc_18650_p25_sococv.xlsx
@@ -1,30 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Desktop\Lab_2\Modle\Project_Lab2\Lab2_parameterest\data\Lab2_data\RLS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C1FDFA-8387-44BD-A76B-0AB0A98D82D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>SOC</t>
+  </si>
+  <si>
+    <t>OCV</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -330,13 +358,200 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0.01</v>
+      </c>
+      <c r="B3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0.05</v>
+      </c>
+      <c r="B4">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.15</v>
+      </c>
+      <c r="B6">
+        <v>3.2250000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.2</v>
+      </c>
+      <c r="B7">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.3</v>
+      </c>
+      <c r="B9">
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.35</v>
+      </c>
+      <c r="B10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.4</v>
+      </c>
+      <c r="B11">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.45</v>
+      </c>
+      <c r="B12">
+        <v>3.6349999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.5</v>
+      </c>
+      <c r="B13">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B14">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.6</v>
+      </c>
+      <c r="B15">
+        <v>3.82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.65</v>
+      </c>
+      <c r="B16">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.7</v>
+      </c>
+      <c r="B17">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.75</v>
+      </c>
+      <c r="B18">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.8</v>
+      </c>
+      <c r="B19">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.85</v>
+      </c>
+      <c r="B20">
+        <v>4.0599999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.9</v>
+      </c>
+      <c r="B21">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.95</v>
+      </c>
+      <c r="B22">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>4.22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>